<commit_message>
adding the styling values to the class variable scope
</commit_message>
<xml_diff>
--- a/create_worksheets/excel_template.xlsx
+++ b/create_worksheets/excel_template.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -36,6 +36,15 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="&lt;property object at 0x0000022C7B2DB4C0&gt;"/>
+    </font>
+    <font>
+      <name val="&lt;property object at 0x0000022C7B2DB510&gt;"/>
+    </font>
+    <font>
+      <name val="&lt;property object at 0x0000022C7B2DB560&gt;"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,11 +73,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1421,7 +1433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C10:O94"/>
+  <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1429,6 +1441,59 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Project: </t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Eurobarometer</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wave: </t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>97.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fieldwork: </t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>19/04 - 16/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Sheet</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Question French</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Question English</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
       <c r="C10" t="n">
         <v>5883</v>

</xml_diff>

<commit_message>
added all global styling variables
</commit_message>
<xml_diff>
--- a/create_worksheets/excel_template.xlsx
+++ b/create_worksheets/excel_template.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -36,15 +36,6 @@
     </font>
     <font>
       <b val="1"/>
-    </font>
-    <font>
-      <name val="&lt;property object at 0x0000022C7B2DB4C0&gt;"/>
-    </font>
-    <font>
-      <name val="&lt;property object at 0x0000022C7B2DB510&gt;"/>
-    </font>
-    <font>
-      <name val="&lt;property object at 0x0000022C7B2DB560&gt;"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,14 +64,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1433,7 +1421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O94"/>
+  <dimension ref="C10:O94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1441,59 +1429,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Project: </t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Eurobarometer</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Wave: </t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>97.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Fieldwork: </t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>19/04 - 16/05/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>Sheet</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Question French</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>Question English</t>
-        </is>
-      </c>
-    </row>
     <row r="10">
       <c r="C10" t="n">
         <v>5883</v>

</xml_diff>

<commit_message>
adding child sheet default styling
</commit_message>
<xml_diff>
--- a/create_worksheets/excel_template.xlsx
+++ b/create_worksheets/excel_template.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -53,6 +53,23 @@
       <b val="1"/>
       <color rgb="00000000"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Ariel"/>
+      <color rgb="000563C1"/>
+      <sz val="10"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Ariel"/>
+      <color rgb="00000000"/>
+      <sz val="8"/>
+    </font>
+    <font>
+      <name val="Ariel"/>
+      <b val="1"/>
+      <color rgb="00000000"/>
+      <sz val="8"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -92,6 +109,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -678,20 +698,58 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C10:O29"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Eurobarometer - 97.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>VOL AA weighted</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>&lt;&lt;Back to content</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
           <t>UE6 EU6</t>
@@ -1538,6 +1596,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5114,20 +5178,58 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C10:O25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Eurobarometer - 97.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>VOL AA weighted</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>&lt;&lt;Back to content</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
           <t>UE6 EU6</t>
@@ -5810,25 +5912,69 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C10:O21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Eurobarometer - 97.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>VOL AA weighted</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>&lt;&lt;Back to content</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
           <t>UE6 EU6</t>
@@ -6347,25 +6493,69 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C10:O25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Eurobarometer - 97.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>VOL AA weighted</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>&lt;&lt;Back to content</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
           <t>UE6 EU6</t>
@@ -7048,25 +7238,69 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C10:O21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Eurobarometer - 97.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>VOL AA weighted</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>&lt;&lt;Back to content</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
           <t>UE6 EU6</t>
@@ -7585,25 +7819,69 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C10:O29"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Eurobarometer - 97.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>VOL AA weighted</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>&lt;&lt;Back to content</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
           <t>UE6 EU6</t>
@@ -8450,25 +8728,69 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C10:O19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Eurobarometer - 97.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>VOL AA weighted</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>&lt;&lt;Back to content</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
           <t>UE6 EU6</t>
@@ -8905,25 +9227,69 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C10:O33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Eurobarometer - 97.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>VOL AA weighted</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="6" t="n"/>
+      <c r="H3" s="6" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>&lt;&lt;Back to content</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
+      <c r="B10" s="8" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
           <t>UE6 EU6</t>
@@ -9934,6 +10300,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the styling ton the content sheet, only the hyperlinks remain
</commit_message>
<xml_diff>
--- a/create_worksheets/excel_template.xlsx
+++ b/create_worksheets/excel_template.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -71,6 +71,11 @@
       <color rgb="00000000"/>
       <sz val="8"/>
     </font>
+    <font>
+      <name val="Ariel"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,13 +110,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -477,7 +482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,171 +527,170 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n"/>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Question</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Question_French</t>
         </is>
       </c>
-      <c r="D5" s="1" t="inlineStr">
+      <c r="C5" s="4" t="inlineStr">
         <is>
           <t>Question_English</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>B. Pays de terrain</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="C6" s="8" t="inlineStr">
         <is>
           <t>B. Fieldwork country</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="inlineStr">
+      <c r="A7" s="8" t="inlineStr">
         <is>
           <t>QB1</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="B7" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">QB1. À quelle fréquence faites-vous du sport ou de l'exercice physique ? Par « faire de l’exercice physique», nous entendons tous les types d’activités physiques que vous pouvez pratiquer dans un contexte sportif ou une infrastructure sportive, comme nager, vous entraîner dans un centre de fitness ou un club sportif, courir dans un parc, etc. </t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="C7" s="8" t="inlineStr">
         <is>
           <t>QB1. How often do you exercise or play sport? By “exercise” we mean any form of physical activity which you do in a sport context or sport-related setting, such as swimming, training in a fitness centre or a sport club, running in the park.</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="inlineStr">
+      <c r="A8" s="8" t="inlineStr">
         <is>
           <t>QB1R</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="B8" s="8" t="inlineStr">
         <is>
           <t xml:space="preserve">QB1R. À quelle fréquence faites-vous du sport ou de l'exercice physique ? Par « faire de l’exercice physique», nous entendons tous les types d’activités physiques que vous pouvez pratiquer dans un contexte sportif ou une infrastructure sportive, comme nager, vous entraîner dans un centre de fitness ou un club sportif, courir dans un parc, etc. </t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="C8" s="8" t="inlineStr">
         <is>
           <t>QB1R. How often do you exercise or play sport? By “exercise” we mean any form of physical activity which you do in a sport context or sport-related setting, such as swimming, training in a fitness centre or a sport club, running in the park.</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="B9" t="inlineStr">
+      <c r="A9" s="8" t="inlineStr">
         <is>
           <t>QB2</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="B9" s="8" t="inlineStr">
         <is>
           <t>QB2. Et à quelle fréquence pratiquez-vous une  autre activité physique qui n'est pas un sport, comme faire du vélo pour vous déplacer d'un lieu à un autre, danser, jardiner, etc. ? Par “autre activité physique”, nous voulons parler d’une activité que vous pratiquez comme loisir ou pour une raison qui n’est pas liée au sport.</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="C9" s="8" t="inlineStr">
         <is>
           <t>QB2. And how often do you engage in other physical activity such as cycling from one place to another, dancing, gardening, etc.? By “other physical activity” we mean physical activity for recreational or non-sport-related reasons.</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" t="inlineStr">
+      <c r="A10" s="8" t="inlineStr">
         <is>
           <t>QB2R</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="B10" s="8" t="inlineStr">
         <is>
           <t>QB2R. Et à quelle fréquence pratiquez-vous une  autre activité physique qui n'est pas un sport, comme faire du vélo pour vous déplacer d'un lieu à un autre, danser, jardiner, etc. ? Par “autre activité physique”, nous voulons parler d’une activité que vous pratiquez comme loisir ou pour une raison qui n’est pas liée au sport.</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="C10" s="8" t="inlineStr">
         <is>
           <t>QB2R. And how often do you engage in other physical activity such as cycling from one place to another, dancing, gardening, etc.? By “other physical activity” we mean physical activity for recreational or non-sport-related reasons.</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="B11" t="inlineStr">
+      <c r="A11" s="8" t="inlineStr">
         <is>
           <t>QB3</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="B11" s="8" t="inlineStr">
         <is>
           <t>QB3. Au cours des 7 derniers jours, combien de jours avez-vous fait un effort physique intense, comme porter des charges lourdes, bêcher, faire de l'aérobic ou rouler vite à vélo ?</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="C11" s="8" t="inlineStr">
         <is>
           <t>QB3. In the last 7 days, on how many days did you do vigorous physical activity like lifting heavy things, digging, aerobics or fast cycling?</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="B12" t="inlineStr">
+      <c r="A12" s="8" t="inlineStr">
         <is>
           <t>QB3R</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="B12" s="8" t="inlineStr">
         <is>
           <t>QB3R. Au cours des 7 derniers jours, combien de jours avez-vous fait un effort physique intense, comme porter des charges lourdes, bêcher, faire de l'aérobic ou rouler vite à vélo ?</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="C12" s="8" t="inlineStr">
         <is>
           <t>QB3R. In the last 7 days, on how many days did you do vigorous physical activity like lifting heavy things, digging, aerobics or fast cycling?</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="B13" t="inlineStr">
+      <c r="A13" s="8" t="inlineStr">
         <is>
           <t>QB4</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="B13" s="8" t="inlineStr">
         <is>
           <t>QB4. En général, les jours où vous faites un effort physique intense, combien de temps y consacrez-vous ?</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="C13" s="8" t="inlineStr">
         <is>
           <t>QB4. In general, on days when you do a vigorous physical activity, how much time do you spend at it?</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="B14" t="inlineStr">
+      <c r="A14" s="8" t="inlineStr">
         <is>
           <t>QB5</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>QB5. Au cours des 7 derniers jours, combien de jours avez-vous fait un effort physique modéré, comme porter des charges légères, faire du vélo à vitesse modérée ou jouer en double au tennis ? Merci de ne pas inclure la marche.</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="C14" s="8" t="inlineStr">
         <is>
           <t>QB5. In the last 7 days, on how many days did you do moderate physical activity like carrying light loads, cycling at normal pace or doubles tennis? Please do not include walking.</t>
         </is>
@@ -710,42 +714,48 @@
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Eurobarometer - 97.3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>VOL AA weighted</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>&lt;&lt;Back to content</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -5190,42 +5200,48 @@
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Eurobarometer - 97.3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>VOL AA weighted</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>&lt;&lt;Back to content</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -5935,42 +5951,48 @@
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Eurobarometer - 97.3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>VOL AA weighted</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>&lt;&lt;Back to content</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -6516,42 +6538,48 @@
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Eurobarometer - 97.3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>VOL AA weighted</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>&lt;&lt;Back to content</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -7261,42 +7289,48 @@
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Eurobarometer - 97.3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>VOL AA weighted</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>&lt;&lt;Back to content</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -7842,42 +7876,48 @@
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Eurobarometer - 97.3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>VOL AA weighted</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>&lt;&lt;Back to content</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -8751,42 +8791,48 @@
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Eurobarometer - 97.3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>VOL AA weighted</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>&lt;&lt;Back to content</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -9250,42 +9296,48 @@
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="I1" s="6" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Eurobarometer - 97.3</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>VOL AA weighted</t>
         </is>
       </c>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Terrain/Fieldwork :  19/04 - 16/05/2022</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="H3" s="5" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>&lt;&lt;Back to content</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Total</t>
         </is>

</xml_diff>

<commit_message>
added additional formatting for the child sheets total label
</commit_message>
<xml_diff>
--- a/create_worksheets/excel_template.xlsx
+++ b/create_worksheets/excel_template.xlsx
@@ -221,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -261,6 +261,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -927,6 +930,7 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="27" customHeight="1"/>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -1015,7 +1019,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -1876,6 +1880,7 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="27" customHeight="1"/>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -1964,7 +1969,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -5966,6 +5971,7 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="27" customHeight="1"/>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -6054,7 +6060,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -6751,6 +6757,7 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="27" customHeight="1"/>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -6839,7 +6846,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -7372,6 +7379,7 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="27" customHeight="1"/>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -7460,7 +7468,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -8157,6 +8165,7 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="27" customHeight="1"/>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -8245,7 +8254,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -8778,6 +8787,7 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="27" customHeight="1"/>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -8866,7 +8876,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -9727,6 +9737,7 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="27" customHeight="1"/>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -9815,7 +9826,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -10266,6 +10277,7 @@
         </is>
       </c>
     </row>
+    <row r="4" ht="27" customHeight="1"/>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -10354,7 +10366,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>Total</t>
         </is>

</xml_diff>

<commit_message>
added further default formatting and values to the template
</commit_message>
<xml_diff>
--- a/create_worksheets/excel_template.xlsx
+++ b/create_worksheets/excel_template.xlsx
@@ -255,15 +255,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,17 +681,17 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="22" t="inlineStr">
+      <c r="A5" s="23" t="inlineStr">
         <is>
           <t>Question</t>
         </is>
       </c>
-      <c r="B5" s="22" t="inlineStr">
+      <c r="B5" s="23" t="inlineStr">
         <is>
           <t>Question_French</t>
         </is>
       </c>
-      <c r="C5" s="22" t="inlineStr">
+      <c r="C5" s="23" t="inlineStr">
         <is>
           <t>Question_English</t>
         </is>
@@ -703,12 +703,12 @@
           <t>B</t>
         </is>
       </c>
-      <c r="B6" s="23" t="inlineStr">
+      <c r="B6" s="24" t="inlineStr">
         <is>
           <t>B. Pays de terrain</t>
         </is>
       </c>
-      <c r="C6" s="23" t="inlineStr">
+      <c r="C6" s="24" t="inlineStr">
         <is>
           <t>B. Fieldwork country</t>
         </is>
@@ -720,12 +720,12 @@
           <t>QB1</t>
         </is>
       </c>
-      <c r="B7" s="23" t="inlineStr">
+      <c r="B7" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">QB1. À quelle fréquence faites-vous du sport ou de l'exercice physique ? Par « faire de l’exercice physique», nous entendons tous les types d’activités physiques que vous pouvez pratiquer dans un contexte sportif ou une infrastructure sportive, comme nager, vous entraîner dans un centre de fitness ou un club sportif, courir dans un parc, etc. </t>
         </is>
       </c>
-      <c r="C7" s="23" t="inlineStr">
+      <c r="C7" s="24" t="inlineStr">
         <is>
           <t>QB1. How often do you exercise or play sport? By “exercise” we mean any form of physical activity which you do in a sport context or sport-related setting, such as swimming, training in a fitness centre or a sport club, running in the park.</t>
         </is>
@@ -737,12 +737,12 @@
           <t>QB1R</t>
         </is>
       </c>
-      <c r="B8" s="23" t="inlineStr">
+      <c r="B8" s="24" t="inlineStr">
         <is>
           <t xml:space="preserve">QB1R. À quelle fréquence faites-vous du sport ou de l'exercice physique ? Par « faire de l’exercice physique», nous entendons tous les types d’activités physiques que vous pouvez pratiquer dans un contexte sportif ou une infrastructure sportive, comme nager, vous entraîner dans un centre de fitness ou un club sportif, courir dans un parc, etc. </t>
         </is>
       </c>
-      <c r="C8" s="23" t="inlineStr">
+      <c r="C8" s="24" t="inlineStr">
         <is>
           <t>QB1R. How often do you exercise or play sport? By “exercise” we mean any form of physical activity which you do in a sport context or sport-related setting, such as swimming, training in a fitness centre or a sport club, running in the park.</t>
         </is>
@@ -754,12 +754,12 @@
           <t>QB2</t>
         </is>
       </c>
-      <c r="B9" s="23" t="inlineStr">
+      <c r="B9" s="24" t="inlineStr">
         <is>
           <t>QB2. Et à quelle fréquence pratiquez-vous une  autre activité physique qui n'est pas un sport, comme faire du vélo pour vous déplacer d'un lieu à un autre, danser, jardiner, etc. ? Par “autre activité physique”, nous voulons parler d’une activité que vous pratiquez comme loisir ou pour une raison qui n’est pas liée au sport.</t>
         </is>
       </c>
-      <c r="C9" s="23" t="inlineStr">
+      <c r="C9" s="24" t="inlineStr">
         <is>
           <t>QB2. And how often do you engage in other physical activity such as cycling from one place to another, dancing, gardening, etc.? By “other physical activity” we mean physical activity for recreational or non-sport-related reasons.</t>
         </is>
@@ -771,12 +771,12 @@
           <t>QB2R</t>
         </is>
       </c>
-      <c r="B10" s="23" t="inlineStr">
+      <c r="B10" s="24" t="inlineStr">
         <is>
           <t>QB2R. Et à quelle fréquence pratiquez-vous une  autre activité physique qui n'est pas un sport, comme faire du vélo pour vous déplacer d'un lieu à un autre, danser, jardiner, etc. ? Par “autre activité physique”, nous voulons parler d’une activité que vous pratiquez comme loisir ou pour une raison qui n’est pas liée au sport.</t>
         </is>
       </c>
-      <c r="C10" s="23" t="inlineStr">
+      <c r="C10" s="24" t="inlineStr">
         <is>
           <t>QB2R. And how often do you engage in other physical activity such as cycling from one place to another, dancing, gardening, etc.? By “other physical activity” we mean physical activity for recreational or non-sport-related reasons.</t>
         </is>
@@ -788,12 +788,12 @@
           <t>QB3</t>
         </is>
       </c>
-      <c r="B11" s="23" t="inlineStr">
+      <c r="B11" s="24" t="inlineStr">
         <is>
           <t>QB3. Au cours des 7 derniers jours, combien de jours avez-vous fait un effort physique intense, comme porter des charges lourdes, bêcher, faire de l'aérobic ou rouler vite à vélo ?</t>
         </is>
       </c>
-      <c r="C11" s="23" t="inlineStr">
+      <c r="C11" s="24" t="inlineStr">
         <is>
           <t>QB3. In the last 7 days, on how many days did you do vigorous physical activity like lifting heavy things, digging, aerobics or fast cycling?</t>
         </is>
@@ -805,12 +805,12 @@
           <t>QB3R</t>
         </is>
       </c>
-      <c r="B12" s="23" t="inlineStr">
+      <c r="B12" s="24" t="inlineStr">
         <is>
           <t>QB3R. Au cours des 7 derniers jours, combien de jours avez-vous fait un effort physique intense, comme porter des charges lourdes, bêcher, faire de l'aérobic ou rouler vite à vélo ?</t>
         </is>
       </c>
-      <c r="C12" s="23" t="inlineStr">
+      <c r="C12" s="24" t="inlineStr">
         <is>
           <t>QB3R. In the last 7 days, on how many days did you do vigorous physical activity like lifting heavy things, digging, aerobics or fast cycling?</t>
         </is>
@@ -822,12 +822,12 @@
           <t>QB4</t>
         </is>
       </c>
-      <c r="B13" s="23" t="inlineStr">
+      <c r="B13" s="24" t="inlineStr">
         <is>
           <t>QB4. En général, les jours où vous faites un effort physique intense, combien de temps y consacrez-vous ?</t>
         </is>
       </c>
-      <c r="C13" s="23" t="inlineStr">
+      <c r="C13" s="24" t="inlineStr">
         <is>
           <t>QB4. In general, on days when you do a vigorous physical activity, how much time do you spend at it?</t>
         </is>
@@ -839,12 +839,12 @@
           <t>QB5</t>
         </is>
       </c>
-      <c r="B14" s="23" t="inlineStr">
+      <c r="B14" s="24" t="inlineStr">
         <is>
           <t>QB5. Au cours des 7 derniers jours, combien de jours avez-vous fait un effort physique modéré, comme porter des charges légères, faire du vélo à vitesse modérée ou jouer en double au tennis ? Merci de ne pas inclure la marche.</t>
         </is>
       </c>
-      <c r="C14" s="23" t="inlineStr">
+      <c r="C14" s="24" t="inlineStr">
         <is>
           <t>QB5. In the last 7 days, on how many days did you do moderate physical activity like carrying light loads, cycling at normal pace or doubles tennis? Please do not include walking.</t>
         </is>
@@ -876,7 +876,11 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -931,6 +935,26 @@
       </c>
     </row>
     <row r="4" ht="27" customHeight="1"/>
+    <row r="5">
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Base: Ensemble</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Base: All Respondents</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
+    </row>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -1019,7 +1043,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -1065,7 +1089,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="21" t="n"/>
+      <c r="B11" s="22" t="n"/>
       <c r="C11" s="14" t="n">
         <v>525</v>
       </c>
@@ -1804,10 +1828,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1"/>
@@ -1826,7 +1854,11 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -1881,6 +1913,26 @@
       </c>
     </row>
     <row r="4" ht="27" customHeight="1"/>
+    <row r="5">
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Base: Ensemble</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Base: All Respondents</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
+    </row>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -1969,7 +2021,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -2015,7 +2067,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="21" t="n"/>
+      <c r="B11" s="22" t="n"/>
       <c r="C11" s="14" t="n">
         <v>0</v>
       </c>
@@ -5895,10 +5947,14 @@
       <c r="O95" s="14" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1"/>
@@ -5917,7 +5973,11 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -5972,6 +6032,26 @@
       </c>
     </row>
     <row r="4" ht="27" customHeight="1"/>
+    <row r="5">
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Base: Ensemble</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Base: All Respondents</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
+    </row>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -6060,7 +6140,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -6106,7 +6186,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="21" t="n"/>
+      <c r="B11" s="22" t="n"/>
       <c r="C11" s="14" t="n">
         <v>360</v>
       </c>
@@ -6681,10 +6761,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1"/>
@@ -6703,7 +6787,11 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -6758,6 +6846,26 @@
       </c>
     </row>
     <row r="4" ht="27" customHeight="1"/>
+    <row r="5">
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Base: Ensemble</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Base: All Respondents</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
+    </row>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -6846,7 +6954,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -6892,7 +7000,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="21" t="n"/>
+      <c r="B11" s="22" t="n"/>
       <c r="C11" s="14" t="n">
         <v>360</v>
       </c>
@@ -7303,10 +7411,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1"/>
@@ -7325,7 +7437,11 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -7380,6 +7496,26 @@
       </c>
     </row>
     <row r="4" ht="27" customHeight="1"/>
+    <row r="5">
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Base: Ensemble</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Base: All Respondents</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
+    </row>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -7468,7 +7604,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -7514,7 +7650,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="21" t="n"/>
+      <c r="B11" s="22" t="n"/>
       <c r="C11" s="14" t="n">
         <v>923</v>
       </c>
@@ -8089,10 +8225,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1"/>
@@ -8111,7 +8251,11 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -8166,6 +8310,26 @@
       </c>
     </row>
     <row r="4" ht="27" customHeight="1"/>
+    <row r="5">
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Base: Ensemble</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Base: All Respondents</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
+    </row>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -8254,7 +8418,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -8300,7 +8464,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="21" t="n"/>
+      <c r="B11" s="22" t="n"/>
       <c r="C11" s="14" t="n">
         <v>923</v>
       </c>
@@ -8711,10 +8875,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1"/>
@@ -8733,7 +8901,11 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -8788,6 +8960,26 @@
       </c>
     </row>
     <row r="4" ht="27" customHeight="1"/>
+    <row r="5">
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Base: Ensemble</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Base: All Respondents</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
+    </row>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -8876,7 +9068,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -8922,7 +9114,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="21" t="n"/>
+      <c r="B11" s="22" t="n"/>
       <c r="C11" s="14" t="n">
         <v>685</v>
       </c>
@@ -9661,10 +9853,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1"/>
@@ -9683,7 +9879,11 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -9738,6 +9938,26 @@
       </c>
     </row>
     <row r="4" ht="27" customHeight="1"/>
+    <row r="5">
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Base: Ensemble</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Base: All Respondents</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
+    </row>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -9826,7 +10046,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -9872,7 +10092,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="21" t="n"/>
+      <c r="B11" s="22" t="n"/>
       <c r="C11" s="14" t="n">
         <v>2047</v>
       </c>
@@ -10201,10 +10421,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1"/>
@@ -10223,7 +10447,11 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -10278,6 +10506,26 @@
       </c>
     </row>
     <row r="4" ht="27" customHeight="1"/>
+    <row r="5">
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Base: Ensemble</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>Base: All Respondents</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="n"/>
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="n"/>
+    </row>
     <row r="8">
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="9" t="n"/>
@@ -10366,7 +10614,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="24" t="inlineStr">
+      <c r="B10" s="21" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -10412,7 +10660,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="21" t="n"/>
+      <c r="B11" s="22" t="n"/>
       <c r="C11" s="14" t="n">
         <v>750</v>
       </c>
@@ -11315,10 +11563,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1"/>

</xml_diff>